<commit_message>
Power point e grafico do excel
</commit_message>
<xml_diff>
--- a/Documentação/FocosIncendioBrasil.xlsx
+++ b/Documentação/FocosIncendioBrasil.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wesley\Desktop\IGNIS\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\ignis\IGNIS\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A6E1C8-5751-49F0-84AC-72F89BE9EA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A19E3E-F180-4C9B-A84C-129AE26E6FA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>-</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Mínimo*</t>
-  </si>
-  <si>
-    <t>Ano</t>
   </si>
   <si>
     <t>Janeiro</t>
@@ -218,6 +215,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA29E00"/>
+      <color rgb="FF833C0B"/>
+      <color rgb="FF760000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -227,6 +231,1447 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="60"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="100"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00">
+                <a:alpha val="85000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="A29E00"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:srgbClr val="A29E00"/>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Janeiro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fevereiro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Março</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maio</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junho</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julho</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Setembro</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Outubro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Novembro</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dezembro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$M$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2553</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1476</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2659</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3366</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5790</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12652</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22774</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42251</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19568</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5113</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BEDA-4029-9F72-0698B1454628}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="833C0B"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:srgbClr val="833C0B"/>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Janeiro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fevereiro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Março</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maio</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junho</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julho</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Setembro</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Outubro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Novembro</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dezembro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4030</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2865</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5213</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2842</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2963</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7258</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13394</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51935</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53234</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25613</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20585</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BEDA-4029-9F72-0698B1454628}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000">
+                <a:alpha val="85000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="760000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:srgbClr val="760000"/>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Janeiro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fevereiro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Março</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maio</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junho</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julho</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Setembro</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Outubro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Novembro</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dezembro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2866</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2657</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4117</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15804</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50694</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>69329</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41468</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13463</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7408</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BEDA-4029-9F72-0698B1454628}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2021</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050">
+                <a:alpha val="85000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:srgbClr val="00B050"/>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Janeiro</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fevereiro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Março</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Maio</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junho</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julho</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Setembro</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Outubro</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Novembro</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dezembro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$M$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2237</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1766</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BEDA-4029-9F72-0698B1454628}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="65"/>
+        <c:shape val="box"/>
+        <c:axId val="581101344"/>
+        <c:axId val="581094272"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="581101344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="581094272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="581094272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="581101344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="288">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr/>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12D38E9C-69BF-4F32-9E92-21884F0C3248}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,8 +1939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,47 +1952,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -791,35 +2234,35 @@
         <v>2595.25</v>
       </c>
       <c r="F7" s="5">
-        <f>AVERAGE(F2:F4)</f>
+        <f t="shared" ref="F7:M7" si="0">AVERAGE(F2:F4)</f>
         <v>3443.6666666666665</v>
       </c>
       <c r="G7" s="5">
-        <f>AVERAGE(G2:G4)</f>
+        <f t="shared" si="0"/>
         <v>6719</v>
       </c>
       <c r="H7" s="5">
-        <f>AVERAGE(H2:H4)</f>
+        <f t="shared" si="0"/>
         <v>13950</v>
       </c>
       <c r="I7" s="5">
-        <f>AVERAGE(I2:I4)</f>
+        <f t="shared" si="0"/>
         <v>41801</v>
       </c>
       <c r="J7" s="5">
-        <f>AVERAGE(J2:J4)</f>
+        <f t="shared" si="0"/>
         <v>54938</v>
       </c>
       <c r="K7" s="3">
-        <f>AVERAGE(K2:K4)</f>
+        <f t="shared" si="0"/>
         <v>28883</v>
       </c>
       <c r="L7" s="5">
-        <f>AVERAGE(L2:L4)</f>
+        <f t="shared" si="0"/>
         <v>15687.333333333334</v>
       </c>
       <c r="M7" s="5">
-        <f>AVERAGE(M2:M4)</f>
+        <f t="shared" si="0"/>
         <v>6740.333333333333</v>
       </c>
       <c r="N7" s="5">
@@ -877,5 +2320,6 @@
   <ignoredErrors>
     <ignoredError sqref="B7:E7 N7" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>